<commit_message>
Separated background and related work, added the table.
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="210" windowWidth="18195" windowHeight="8895" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="480" yWindow="210" windowWidth="18195" windowHeight="8895" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,17 @@
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="cont1_whenEatenVsEnteredTable" sheetId="12" r:id="rId12"/>
     <sheet name="cont1_meanStartsPerDay" sheetId="13" r:id="rId13"/>
+    <sheet name="chap2" sheetId="14" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="655">
   <si>
     <t>User Search Request</t>
   </si>
@@ -2051,6 +2052,387 @@
   <si>
     <t xml:space="preserve">Min: </t>
   </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Challenges</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Goal/purpose</t>
+  </si>
+  <si>
+    <t>(Glanz et al. 2006)</t>
+  </si>
+  <si>
+    <t>Women in Diet Modifcation arm of Women’s health Initiative.</t>
+  </si>
+  <si>
+    <t>1 month</t>
+  </si>
+  <si>
+    <t>Entries made a mean of 5 days/wk; half ppts made entries 6-7 days/wk. 62% of of days, entries were made &gt;=3 different times.</t>
+  </si>
+  <si>
+    <t>Support participants in following a particular diet plan</t>
+  </si>
+  <si>
+    <t>(L. E. Burke et al. 2011)</t>
+  </si>
+  <si>
+    <t>Overweight/obese (BMI), no medical conditions,</t>
+  </si>
+  <si>
+    <t>6 months</t>
+  </si>
+  <si>
+    <t>SMART trial, 6 mth outcomes</t>
+  </si>
+  <si>
+    <t>(Acharya et al. 2011)</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>6 mths</t>
+  </si>
+  <si>
+    <t>SMART trial, 6 mth outcomes, secondary analysis</t>
+  </si>
+  <si>
+    <t>(Arsand et al. 2007)</t>
+  </si>
+  <si>
+    <t>12 &amp; 20</t>
+  </si>
+  <si>
+    <t>12 w/ diabetes, 20 general</t>
+  </si>
+  <si>
+    <t>Feedback about the design of the tool (interface)</t>
+  </si>
+  <si>
+    <t>(Bojic et al. 2009)</t>
+  </si>
+  <si>
+    <t>(ages 55-70)</t>
+  </si>
+  <si>
+    <t>Self built</t>
+  </si>
+  <si>
+    <t>Feedback about the design of the tool/interface</t>
+  </si>
+  <si>
+    <t>(P. Jarvinen et al. 2008)</t>
+  </si>
+  <si>
+    <t>“People liked it”</t>
+  </si>
+  <si>
+    <t>Self-built</t>
+  </si>
+  <si>
+    <t>Feedback about the use of the entire system</t>
+  </si>
+  <si>
+    <t>(Mattila et al. 2008)</t>
+  </si>
+  <si>
+    <t>Overweight, had S60 phone</t>
+  </si>
+  <si>
+    <t>3 months</t>
+  </si>
+  <si>
+    <t>Test ability of WD to support CBT-based weight management</t>
+  </si>
+  <si>
+    <t>(Kozakai et al. 2006)</t>
+  </si>
+  <si>
+    <t>Grad student volunteer</t>
+  </si>
+  <si>
+    <t>2 mths</t>
+  </si>
+  <si>
+    <t>Self-built; included scale, blood pressure meter, diet diary</t>
+  </si>
+  <si>
+    <t>Test the tool</t>
+  </si>
+  <si>
+    <t>(Reddy et al. 2007)</t>
+  </si>
+  <si>
+    <t>2 wks</t>
+  </si>
+  <si>
+    <t>Eh, was just image collection analyzed in terms of food/meals</t>
+  </si>
+  <si>
+    <t>Merely collected images + context, no self-monitoring or reflection</t>
+  </si>
+  <si>
+    <t>DietSense prototype, Nokia N80 phone, captured images + audio + context, location every 10 seconds</t>
+  </si>
+  <si>
+    <t>Evaluate potential usefulness for DietSense, collect data to inform future development.</t>
+  </si>
+  <si>
+    <t>(Silva et al. 2011)</t>
+  </si>
+  <si>
+    <t>“Several users”</t>
+  </si>
+  <si>
+    <t>“Several weeks”</t>
+  </si>
+  <si>
+    <t>“There was pretty good feedback from users.”</t>
+  </si>
+  <si>
+    <t>“Several</t>
+  </si>
+  <si>
+    <t>Self-developed Android-based system</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (Tsai et al. 2007)</t>
+  </si>
+  <si>
+    <t>PmEB</t>
+  </si>
+  <si>
+    <t>Clinically Overweight (BMI&gt;=25)</t>
+  </si>
+  <si>
+    <t>(Wang et al. 2006)</t>
+  </si>
+  <si>
+    <t>Students majoring in nutrition; “highly motivated”J</t>
+  </si>
+  <si>
+    <t>2 days, 6 mths apart</t>
+  </si>
+  <si>
+    <t>Test the Wellnavi approach, of taking photos &amp; time to enter a record, versus the weighed record or recall</t>
+  </si>
+  <si>
+    <t>(Long et al. 2012)</t>
+  </si>
+  <si>
+    <t>MyPyramid tracker (website) compared to mobile phone food photographs.</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>While photos were helpful, they weren’t perfect, serving sizes were still an issue</t>
+  </si>
+  <si>
+    <t>Whether cell phone photos are an effective memory prompt for using MyPyramid tracker</t>
+  </si>
+  <si>
+    <t>(Atienza et al. 2008)</t>
+  </si>
+  <si>
+    <t>Compared PDA-based assessment</t>
+  </si>
+  <si>
+    <t>Adults &gt;=50yrs</t>
+  </si>
+  <si>
+    <t>8 wks</t>
+  </si>
+  <si>
+    <t>PDA-based, 43-question assessment (triggered 2x/day)</t>
+  </si>
+  <si>
+    <t>(Yon et al. 2007)</t>
+  </si>
+  <si>
+    <t>(71 PDA, 115 paper control)</t>
+  </si>
+  <si>
+    <t>Overweight, participating in weight control program</t>
+  </si>
+  <si>
+    <t>CalorieKing Diet Diary</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Number of Participants</t>
+  </si>
+  <si>
+    <t>Target Population</t>
+  </si>
+  <si>
+    <t>Database Information</t>
+  </si>
+  <si>
+    <t>Custom developed; db built from program materials, ~300 items.Tracked fat, servings of fruit, veggie &amp; grains.</t>
+  </si>
+  <si>
+    <t>Adherence: PDA+FB=90%, PDA=80%, PR=55%</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PDA (w/ &amp; w/o feedback) versus PR  (paper); of the calorie goal was recorded for the week.; Daily self-monitoring, group sessions, daily dietary goals (calories), weekly exercise goals; Adherence to dietary self-monitoring was counted if at least 50% </t>
+  </si>
+  <si>
+    <t>Same as above; DietmatePro on Palm PDAs</t>
+  </si>
+  <si>
+    <t>Targeted for Type 2 diabetes; 4 “focus groups”, all the same people; No in situ eval</t>
+  </si>
+  <si>
+    <t>No in situ eval; Diabetes focus.</t>
+  </si>
+  <si>
+    <t>HyperFit, web &amp; mobile apps.; 4 trials overall.</t>
+  </si>
+  <si>
+    <t>97 individual users;9 nutritionists;5 groups/39 participants;</t>
+  </si>
+  <si>
+    <t>First 2 trials: people interested in weight management; Third trial, tool for support in a weight management group; Fourth, as a tool for nutrition counseling.</t>
+  </si>
+  <si>
+    <t>Individuals: 2 weeks; Counseling: 3 wks; Groups: tasks of tracking for 2-3 days at a time.</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nutritional data; ·         Technology in infancy; ·         Creating records in food &amp; exercise diary were too time consuming/challenging.</t>
+    </r>
+  </si>
+  <si>
+    <t>Importance and input frequency of food &amp; drink decreased dramatically over the course of the study. People felt it important to be careful in observing at the beginning, but less so later.;Importance of recording weight increased over the study.</t>
+  </si>
+  <si>
+    <t>Wellness Diary/self built;Triage approach</t>
+  </si>
+  <si>
+    <t>Wellness Diary; (weight management study); 1.5 hr lecture on weight change via CBT</t>
+  </si>
+  <si>
+    <t>LOSERS made more entries in all categories than OTHERS group; 79% thought it would help them lose weight.64% wanted to continue using it</t>
+  </si>
+  <si>
+    <t>DietSense; Taking &amp; dealing with images of food eaten</t>
+  </si>
+  <si>
+    <t>SapoFitness; Reflects little insight of persuasive design; Doesn’t identify details of “database testing”</t>
+  </si>
+  <si>
+    <t>“Several scenarios were experimented and the system performed very well, as expected. These experiments included communication with food database, daily food inserted, behaviour of the users, profile changes, and motivation of the users to use the 379 application.”</t>
+  </si>
+  <si>
+    <t>PmEB; Food is chosen from a list of prechosen foods on the web; Paper, PmEB, PmEB+reminders</t>
+  </si>
+  <si>
+    <t>WellNavi.; Students kept 1 weighed food records, took photos, + 24 hr recall.</t>
+  </si>
+  <si>
+    <t>Veggie intake in the PDA group increased more.; Ppts completed ~51% of the assessments.; Week 1=75%, Week 8=40%.</t>
+  </si>
+  <si>
+    <t>Whether PDA intervention increases veggie &amp; whole grain intake; (CHART-D program)</t>
+  </si>
+  <si>
+    <t>6-mth behavioral strategies/self-management skills weight loss program. Weekly meetings.; “First few weeks” were spent trouble-shooting use of software. Positive (personalized) feedback occurred on a weekly basis.</t>
+  </si>
+  <si>
+    <t>Compared to previous study using similar protocol but with pencil/paper, and didn’t find a difference.Overall, those who self-monitored lost more.</t>
+  </si>
+  <si>
+    <t>26% of PDA users liked the “ease of use of entering food and exercise data”, 44% reported they disliked the PDA/software (because they couldn’t find food they eat and couldn’t see the screen). Even with support, ppts still had trouble navigating the software and finding foods.</t>
+  </si>
+  <si>
+    <t>~300 items</t>
+  </si>
+  <si>
+    <t>USDA db, 5000-6000 items</t>
+  </si>
+  <si>
+    <t>2500 items</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>607 w/o barcode, 805 w/ barcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food sometimes wasn’t in the database; Selected foods via menu or barcode scan. </t>
+  </si>
+  <si>
+    <t>Not reported</t>
+  </si>
+  <si>
+    <t>750 items</t>
+  </si>
+  <si>
+    <t>None, paper and pencil</t>
+  </si>
+  <si>
+    <t>USDA db, ~6000 items</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Not reported in paper; current CalorieKing Diet Diary states 50,000 records</t>
+  </si>
+  <si>
+    <t>Fukuo</t>
+  </si>
+  <si>
+    <t>PDA, proprietary w/ photos for serving sizes</t>
+  </si>
+  <si>
+    <t>44 w/o diabetes, 16 w/ diabetes</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>PDA agrees w/ recall</t>
+  </si>
 </sst>
 </file>
 
@@ -2059,7 +2441,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2191,6 +2573,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -2638,7 +3033,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2788,6 +3183,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2806,6 +3212,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2813,9 +3222,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2830,23 +3236,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3520,11 +3930,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44123648"/>
-        <c:axId val="238592576"/>
+        <c:axId val="199597568"/>
+        <c:axId val="200815104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44123648"/>
+        <c:axId val="199597568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3546,7 +3956,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -3562,7 +3971,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238592576"/>
+        <c:crossAx val="200815104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3570,7 +3979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="238592576"/>
+        <c:axId val="200815104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3593,7 +4002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3610,14 +4018,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44123648"/>
+        <c:crossAx val="199597568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4017,14 +4424,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C8" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4">
   <autoFilter ref="A1:C8"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Component" dataDxfId="2"/>
-    <tableColumn id="2" name="Points" dataDxfId="1"/>
-    <tableColumn id="3" name="Serving goal" dataDxfId="0"/>
+    <tableColumn id="1" name="Component" dataDxfId="3"/>
+    <tableColumn id="2" name="Points" dataDxfId="2"/>
+    <tableColumn id="3" name="Serving goal" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:K17" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K17"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Reference"/>
+    <tableColumn id="2" name="Column1"/>
+    <tableColumn id="3" name="Number of Participants"/>
+    <tableColumn id="4" name="Target Population"/>
+    <tableColumn id="5" name="Duration"/>
+    <tableColumn id="6" name="Results"/>
+    <tableColumn id="7" name="Challenges"/>
+    <tableColumn id="8" name="Column2"/>
+    <tableColumn id="9" name="Instrument"/>
+    <tableColumn id="10" name="Goal/purpose"/>
+    <tableColumn id="11" name="Database Information"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4341,10 +4768,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="65" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -4352,31 +4779,31 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
-      <c r="B3" s="59"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="66"/>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="59"/>
+      <c r="A4" s="63"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="60"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="65" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -4384,8 +4811,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="60"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
@@ -11192,10 +11619,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="55" t="s">
         <v>512</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="56" t="s">
         <v>513</v>
       </c>
       <c r="C3" t="s">
@@ -11206,10 +11633,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="57" t="s">
         <v>522</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="58" t="s">
         <v>516</v>
       </c>
       <c r="C4">
@@ -11226,8 +11653,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
-      <c r="B5" s="73" t="s">
+      <c r="A5" s="57"/>
+      <c r="B5" s="59" t="s">
         <v>517</v>
       </c>
       <c r="C5">
@@ -11244,8 +11671,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="73" t="s">
+      <c r="A6" s="57"/>
+      <c r="B6" s="59" t="s">
         <v>518</v>
       </c>
       <c r="C6">
@@ -11262,8 +11689,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="73" t="s">
+      <c r="A7" s="57"/>
+      <c r="B7" s="59" t="s">
         <v>519</v>
       </c>
       <c r="C7">
@@ -11280,8 +11707,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73" t="s">
+      <c r="A8" s="57"/>
+      <c r="B8" s="59" t="s">
         <v>520</v>
       </c>
       <c r="C8">
@@ -11298,8 +11725,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="75" t="s">
+      <c r="A9" s="60"/>
+      <c r="B9" s="61" t="s">
         <v>521</v>
       </c>
       <c r="C9">
@@ -11316,10 +11743,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="57" t="s">
         <v>523</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="58" t="s">
         <v>516</v>
       </c>
       <c r="C10">
@@ -11336,8 +11763,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="73" t="s">
+      <c r="A11" s="57"/>
+      <c r="B11" s="59" t="s">
         <v>517</v>
       </c>
       <c r="C11">
@@ -11354,8 +11781,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="73" t="s">
+      <c r="A12" s="57"/>
+      <c r="B12" s="59" t="s">
         <v>518</v>
       </c>
       <c r="C12">
@@ -11372,8 +11799,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="73" t="s">
+      <c r="A13" s="57"/>
+      <c r="B13" s="59" t="s">
         <v>519</v>
       </c>
       <c r="C13">
@@ -11390,8 +11817,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="57"/>
+      <c r="B14" s="59" t="s">
         <v>520</v>
       </c>
       <c r="C14">
@@ -11408,8 +11835,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="74"/>
-      <c r="B15" s="75" t="s">
+      <c r="A15" s="60"/>
+      <c r="B15" s="61" t="s">
         <v>521</v>
       </c>
       <c r="C15">
@@ -11426,10 +11853,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="57" t="s">
         <v>524</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="58" t="s">
         <v>516</v>
       </c>
       <c r="C16">
@@ -11446,8 +11873,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="73" t="s">
+      <c r="A17" s="57"/>
+      <c r="B17" s="59" t="s">
         <v>517</v>
       </c>
       <c r="C17">
@@ -11464,8 +11891,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="73" t="s">
+      <c r="A18" s="57"/>
+      <c r="B18" s="59" t="s">
         <v>518</v>
       </c>
       <c r="C18">
@@ -11482,8 +11909,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="71"/>
-      <c r="B19" s="73" t="s">
+      <c r="A19" s="57"/>
+      <c r="B19" s="59" t="s">
         <v>519</v>
       </c>
       <c r="C19">
@@ -11500,8 +11927,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
-      <c r="B20" s="73" t="s">
+      <c r="A20" s="57"/>
+      <c r="B20" s="59" t="s">
         <v>520</v>
       </c>
       <c r="C20">
@@ -11518,8 +11945,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
-      <c r="B21" s="75" t="s">
+      <c r="A21" s="60"/>
+      <c r="B21" s="61" t="s">
         <v>521</v>
       </c>
       <c r="C21">
@@ -11536,10 +11963,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="57" t="s">
         <v>525</v>
       </c>
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="58" t="s">
         <v>516</v>
       </c>
       <c r="C22">
@@ -11556,8 +11983,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="73" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="59" t="s">
         <v>517</v>
       </c>
       <c r="C23">
@@ -11574,8 +12001,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
-      <c r="B24" s="73" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="59" t="s">
         <v>518</v>
       </c>
       <c r="C24">
@@ -11592,8 +12019,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="71"/>
-      <c r="B25" s="73" t="s">
+      <c r="A25" s="57"/>
+      <c r="B25" s="59" t="s">
         <v>519</v>
       </c>
       <c r="C25">
@@ -11610,8 +12037,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="73" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="59" t="s">
         <v>520</v>
       </c>
       <c r="C26">
@@ -11628,8 +12055,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="74"/>
-      <c r="B27" s="75" t="s">
+      <c r="A27" s="60"/>
+      <c r="B27" s="61" t="s">
         <v>521</v>
       </c>
       <c r="C27">
@@ -11646,10 +12073,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="57" t="s">
         <v>526</v>
       </c>
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="58" t="s">
         <v>516</v>
       </c>
       <c r="C28">
@@ -11666,8 +12093,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
-      <c r="B29" s="73" t="s">
+      <c r="A29" s="57"/>
+      <c r="B29" s="59" t="s">
         <v>517</v>
       </c>
       <c r="C29">
@@ -11684,8 +12111,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
-      <c r="B30" s="73" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="59" t="s">
         <v>518</v>
       </c>
       <c r="C30">
@@ -11702,8 +12129,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
-      <c r="B31" s="73" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="59" t="s">
         <v>519</v>
       </c>
       <c r="C31">
@@ -11720,8 +12147,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
-      <c r="B32" s="73" t="s">
+      <c r="A32" s="57"/>
+      <c r="B32" s="59" t="s">
         <v>520</v>
       </c>
       <c r="C32">
@@ -11738,8 +12165,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="74"/>
-      <c r="B33" s="75" t="s">
+      <c r="A33" s="60"/>
+      <c r="B33" s="61" t="s">
         <v>521</v>
       </c>
       <c r="C33">
@@ -11756,10 +12183,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="57" t="s">
         <v>527</v>
       </c>
-      <c r="B34" s="73"/>
+      <c r="B34" s="59"/>
       <c r="C34">
         <f>[1]EatenTimeOverTime!AL34</f>
         <v>18</v>
@@ -11783,7 +12210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
@@ -12323,6 +12750,525 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2700" topLeftCell="C1" activePane="topRight"/>
+      <selection activeCell="B17" sqref="B17"/>
+      <selection pane="topRight" activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="76" t="s">
+        <v>607</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>608</v>
+      </c>
+      <c r="D1" s="76" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="76" t="s">
+        <v>535</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>536</v>
+      </c>
+      <c r="H1" s="76" t="s">
+        <v>614</v>
+      </c>
+      <c r="I1" s="76" t="s">
+        <v>537</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>538</v>
+      </c>
+      <c r="K1" s="77" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="164.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76">
+        <v>33</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>540</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>541</v>
+      </c>
+      <c r="F2" s="76" t="s">
+        <v>542</v>
+      </c>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76" t="s">
+        <v>611</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>543</v>
+      </c>
+      <c r="K2" s="78" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="76" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>615</v>
+      </c>
+      <c r="C3" s="76">
+        <v>210</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>545</v>
+      </c>
+      <c r="E3" s="76" t="s">
+        <v>546</v>
+      </c>
+      <c r="F3" s="76" t="s">
+        <v>612</v>
+      </c>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76" t="s">
+        <v>547</v>
+      </c>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="57" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76" t="s">
+        <v>548</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>616</v>
+      </c>
+      <c r="C4" s="76">
+        <v>210</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>549</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>550</v>
+      </c>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76" t="s">
+        <v>551</v>
+      </c>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="57"/>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="76" t="s">
+        <v>552</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>617</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>553</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>554</v>
+      </c>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76" t="s">
+        <v>555</v>
+      </c>
+      <c r="K5" s="57"/>
+    </row>
+    <row r="6" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="76" t="s">
+        <v>556</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>618</v>
+      </c>
+      <c r="C6" s="76">
+        <v>32</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>557</v>
+      </c>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76" t="s">
+        <v>558</v>
+      </c>
+      <c r="J6" s="76" t="s">
+        <v>559</v>
+      </c>
+      <c r="K6" s="57"/>
+    </row>
+    <row r="7" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="76" t="s">
+        <v>560</v>
+      </c>
+      <c r="B7" s="76" t="s">
+        <v>619</v>
+      </c>
+      <c r="C7" s="76" t="s">
+        <v>620</v>
+      </c>
+      <c r="D7" s="76" t="s">
+        <v>621</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>622</v>
+      </c>
+      <c r="F7" s="76" t="s">
+        <v>561</v>
+      </c>
+      <c r="G7" s="79" t="s">
+        <v>623</v>
+      </c>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76" t="s">
+        <v>562</v>
+      </c>
+      <c r="J7" s="76" t="s">
+        <v>563</v>
+      </c>
+      <c r="K7" s="57" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="76" t="s">
+        <v>564</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>626</v>
+      </c>
+      <c r="C8" s="76">
+        <v>29</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>565</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>566</v>
+      </c>
+      <c r="F8" s="76" t="s">
+        <v>627</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>624</v>
+      </c>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76" t="s">
+        <v>625</v>
+      </c>
+      <c r="J8" s="76" t="s">
+        <v>567</v>
+      </c>
+      <c r="K8" s="57" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="76" t="s">
+        <v>568</v>
+      </c>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76">
+        <v>1</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>569</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>570</v>
+      </c>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76" t="s">
+        <v>643</v>
+      </c>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76" t="s">
+        <v>571</v>
+      </c>
+      <c r="J9" s="76" t="s">
+        <v>572</v>
+      </c>
+      <c r="K9" s="57" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="76" t="s">
+        <v>573</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>628</v>
+      </c>
+      <c r="C10" s="76">
+        <v>6</v>
+      </c>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76" t="s">
+        <v>574</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>575</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>576</v>
+      </c>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76" t="s">
+        <v>577</v>
+      </c>
+      <c r="J10" s="76" t="s">
+        <v>578</v>
+      </c>
+      <c r="K10" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+      <c r="A11" s="76" t="s">
+        <v>579</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>629</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>580</v>
+      </c>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76" t="s">
+        <v>581</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>582</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>583</v>
+      </c>
+      <c r="H11" s="76"/>
+      <c r="I11" s="76" t="s">
+        <v>584</v>
+      </c>
+      <c r="J11" s="76" t="s">
+        <v>630</v>
+      </c>
+      <c r="K11" s="57" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="76" t="s">
+        <v>585</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>631</v>
+      </c>
+      <c r="C12" s="76">
+        <v>15</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>587</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>541</v>
+      </c>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76" t="s">
+        <v>586</v>
+      </c>
+      <c r="J12" s="76"/>
+      <c r="K12" s="57" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="76" t="s">
+        <v>588</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>632</v>
+      </c>
+      <c r="C13" s="76">
+        <v>28</v>
+      </c>
+      <c r="D13" s="76" t="s">
+        <v>589</v>
+      </c>
+      <c r="E13" s="76" t="s">
+        <v>590</v>
+      </c>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="76" t="s">
+        <v>591</v>
+      </c>
+      <c r="K13" s="57" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="76" t="s">
+        <v>592</v>
+      </c>
+      <c r="B14" s="76" t="s">
+        <v>593</v>
+      </c>
+      <c r="C14" s="76">
+        <v>69</v>
+      </c>
+      <c r="D14" s="76" t="s">
+        <v>594</v>
+      </c>
+      <c r="E14" s="76" t="s">
+        <v>595</v>
+      </c>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76" t="s">
+        <v>596</v>
+      </c>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="76" t="s">
+        <v>597</v>
+      </c>
+      <c r="K14" s="57" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="76" t="s">
+        <v>598</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>599</v>
+      </c>
+      <c r="C15" s="76">
+        <v>27</v>
+      </c>
+      <c r="D15" s="76" t="s">
+        <v>600</v>
+      </c>
+      <c r="E15" s="76" t="s">
+        <v>601</v>
+      </c>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76" t="s">
+        <v>633</v>
+      </c>
+      <c r="H15" s="76"/>
+      <c r="I15" s="76" t="s">
+        <v>602</v>
+      </c>
+      <c r="J15" s="76" t="s">
+        <v>634</v>
+      </c>
+      <c r="K15" s="57" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="A16" s="76" t="s">
+        <v>603</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>635</v>
+      </c>
+      <c r="C16" s="76" t="s">
+        <v>604</v>
+      </c>
+      <c r="D16" s="76" t="s">
+        <v>605</v>
+      </c>
+      <c r="E16" s="76" t="s">
+        <v>546</v>
+      </c>
+      <c r="F16" s="76" t="s">
+        <v>636</v>
+      </c>
+      <c r="G16" s="76" t="s">
+        <v>637</v>
+      </c>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76" t="s">
+        <v>606</v>
+      </c>
+      <c r="K16" s="57" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>650</v>
+      </c>
+      <c r="C17" t="s">
+        <v>651</v>
+      </c>
+      <c r="D17" t="s">
+        <v>652</v>
+      </c>
+      <c r="E17" t="s">
+        <v>653</v>
+      </c>
+      <c r="F17" t="s">
+        <v>654</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -12986,24 +13932,24 @@
       <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="69" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="68" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="68"/>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="36"/>
@@ -13032,42 +13978,42 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66" t="s">
+      <c r="B11" s="72"/>
+      <c r="C11" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="D11" s="74" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="67"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="74"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="69" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="68" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="61"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="68"/>
     </row>
     <row r="15" spans="1:4" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
@@ -13084,28 +14030,28 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="68" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="61"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="64"/>
+      <c r="A17" s="69"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="68"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="61"/>
-      <c r="B18" s="65" t="s">
+      <c r="A18" s="69"/>
+      <c r="B18" s="72" t="s">
         <v>103</v>
       </c>
       <c r="C18" s="32" t="s">
@@ -13116,8 +14062,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="32" t="s">
         <v>94</v>
       </c>
@@ -13126,8 +14072,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="69"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="32" t="s">
         <v>104</v>
       </c>
@@ -13150,24 +14096,24 @@
       <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="61" t="s">
+      <c r="A23" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="71" t="s">
         <v>104</v>
       </c>
-      <c r="D23" s="64" t="s">
+      <c r="D23" s="68" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="64"/>
+      <c r="A24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="68"/>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
@@ -13249,6 +14195,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="D23:D24"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
@@ -13263,14 +14217,6 @@
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13862,42 +14808,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="75" t="s">
         <v>178</v>
       </c>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68" t="s">
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68" t="s">
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
       <c r="E2" s="53"/>
-      <c r="F2" s="68" t="s">
+      <c r="F2" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
       <c r="I2" s="53"/>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="75" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -19846,7 +20792,7 @@
         <v>0</v>
       </c>
       <c r="D258">
-        <f t="shared" ref="D258:D321" si="8">C258+B258</f>
+        <f t="shared" ref="D258:D309" si="8">C258+B258</f>
         <v>0</v>
       </c>
       <c r="E258">

</xml_diff>